<commit_message>
Fixed wrong 14C values
</commit_message>
<xml_diff>
--- a/ISRaD_data_files/Leavitt_2007.xlsx
+++ b/ISRaD_data_files/Leavitt_2007.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20366"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\PhD\ISRaD\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{771DD274-0D46-4384-BE47-B2738165D398}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26280" windowHeight="12480" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8772" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
     <sheet name="incubation" sheetId="8" r:id="rId8"/>
     <sheet name="controlled vocabulary" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2370" uniqueCount="1257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2359" uniqueCount="1256">
   <si>
     <t>entry_name</t>
   </si>
@@ -3788,9 +3794,6 @@
   </si>
   <si>
     <t>Reported as "modern"</t>
-  </si>
-  <si>
-    <t>Inf</t>
   </si>
   <si>
     <t>frc_fraction_modern</t>
@@ -3805,7 +3808,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3923,15 +3926,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_layer" xfId="3"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal_layer" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -4213,14 +4224,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4270,7 +4281,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4317,7 +4328,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -4355,7 +4366,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -4408,19 +4419,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4443,7 +4454,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4466,7 +4477,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -4483,7 +4494,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -4500,7 +4511,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -4517,7 +4528,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -4534,7 +4545,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -4551,7 +4562,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -4568,7 +4579,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -4585,7 +4596,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -4602,7 +4613,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -4619,7 +4630,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -4636,7 +4647,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -4653,7 +4664,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -4670,7 +4681,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -4702,14 +4713,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4819,7 +4830,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4929,7 +4940,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -5024,7 +5035,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -5050,7 +5061,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -5076,7 +5087,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -5102,7 +5113,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -5128,7 +5139,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -5154,7 +5165,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -5180,7 +5191,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -5206,7 +5217,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -5232,7 +5243,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -5258,7 +5269,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -5284,7 +5295,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -5310,7 +5321,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -5348,14 +5359,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AK3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5468,7 +5479,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5578,7 +5589,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -5670,16 +5681,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:CT112"/>
   <sheetViews>
-    <sheetView topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="BC4" sqref="BC4:BC14"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="BB12" sqref="BB12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:98">
+    <row r="1" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5975,7 +5986,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="2" spans="1:98">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -6271,7 +6282,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="3" spans="1:98">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -6510,7 +6521,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="4" spans="1:98">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -6541,11 +6552,8 @@
       <c r="AO4" t="s">
         <v>499</v>
       </c>
-      <c r="BC4" t="s">
-        <v>1253</v>
-      </c>
-    </row>
-    <row r="5" spans="1:98">
+    </row>
+    <row r="5" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -6576,11 +6584,8 @@
       <c r="AO5" t="s">
         <v>502</v>
       </c>
-      <c r="BC5" t="s">
-        <v>1253</v>
-      </c>
-    </row>
-    <row r="6" spans="1:98">
+    </row>
+    <row r="6" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -6611,11 +6616,8 @@
       <c r="AO6" t="s">
         <v>505</v>
       </c>
-      <c r="BC6" t="s">
-        <v>1253</v>
-      </c>
-    </row>
-    <row r="7" spans="1:98">
+    </row>
+    <row r="7" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -6646,11 +6648,8 @@
       <c r="AO7" t="s">
         <v>509</v>
       </c>
-      <c r="BC7" t="s">
-        <v>1253</v>
-      </c>
-    </row>
-    <row r="8" spans="1:98">
+    </row>
+    <row r="8" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -6681,11 +6680,8 @@
       <c r="AO8" t="s">
         <v>513</v>
       </c>
-      <c r="BC8" t="s">
-        <v>1253</v>
-      </c>
-    </row>
-    <row r="9" spans="1:98">
+    </row>
+    <row r="9" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -6716,11 +6712,8 @@
       <c r="AO9" t="s">
         <v>516</v>
       </c>
-      <c r="BC9" t="s">
-        <v>1253</v>
-      </c>
-    </row>
-    <row r="10" spans="1:98">
+    </row>
+    <row r="10" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -6751,11 +6744,8 @@
       <c r="AO10" t="s">
         <v>518</v>
       </c>
-      <c r="BC10" t="s">
-        <v>1253</v>
-      </c>
-    </row>
-    <row r="11" spans="1:98">
+    </row>
+    <row r="11" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -6786,11 +6776,8 @@
       <c r="AO11" t="s">
         <v>522</v>
       </c>
-      <c r="BC11" t="s">
-        <v>1253</v>
-      </c>
-    </row>
-    <row r="12" spans="1:98">
+    </row>
+    <row r="12" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -6821,11 +6808,8 @@
       <c r="AO12" t="s">
         <v>525</v>
       </c>
-      <c r="BC12" t="s">
-        <v>1253</v>
-      </c>
-    </row>
-    <row r="13" spans="1:98">
+    </row>
+    <row r="13" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -6856,11 +6840,8 @@
       <c r="AO13" t="s">
         <v>527</v>
       </c>
-      <c r="BC13" t="s">
-        <v>1253</v>
-      </c>
-    </row>
-    <row r="14" spans="1:98">
+    </row>
+    <row r="14" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -6891,11 +6872,8 @@
       <c r="AO14" t="s">
         <v>529</v>
       </c>
-      <c r="BC14" t="s">
-        <v>1253</v>
-      </c>
-    </row>
-    <row r="15" spans="1:98">
+    </row>
+    <row r="15" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -6930,7 +6908,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:98">
+    <row r="16" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -6965,7 +6943,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:56">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -7000,7 +6978,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:56">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -7035,7 +7013,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:56">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -7070,7 +7048,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:56">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -7105,7 +7083,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:56">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -7140,7 +7118,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:56">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -7175,7 +7153,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:56">
+    <row r="23" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -7210,7 +7188,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:56">
+    <row r="24" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -7245,7 +7223,7 @@
         <v>6.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:56">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -7280,7 +7258,7 @@
         <v>6.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:56">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -7315,7 +7293,7 @@
         <v>1.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:56">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -7350,7 +7328,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:56">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -7385,7 +7363,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:56">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -7420,7 +7398,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:56">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -7455,7 +7433,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:56">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -7490,7 +7468,7 @@
         <v>1.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:56">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -7525,7 +7503,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:56">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -7560,7 +7538,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:56">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -7595,7 +7573,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:56">
+    <row r="35" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -7630,7 +7608,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="36" spans="1:56">
+    <row r="36" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -7665,7 +7643,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:56">
+    <row r="37" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -7700,7 +7678,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:56">
+    <row r="38" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -7735,7 +7713,7 @@
         <v>1.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:56">
+    <row r="39" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -7770,7 +7748,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:56">
+    <row r="40" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -7805,7 +7783,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:56">
+    <row r="41" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -7840,7 +7818,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:56">
+    <row r="42" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -7875,7 +7853,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:56">
+    <row r="43" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -7910,7 +7888,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:56">
+    <row r="44" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -7945,7 +7923,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:56">
+    <row r="45" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -7980,7 +7958,7 @@
         <v>1.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:56">
+    <row r="46" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -8015,7 +7993,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="47" spans="1:56">
+    <row r="47" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -8050,7 +8028,7 @@
         <v>1.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:56">
+    <row r="48" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>43</v>
       </c>
@@ -8085,7 +8063,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:56">
+    <row r="49" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -8120,7 +8098,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:56">
+    <row r="50" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -8155,7 +8133,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:56">
+    <row r="51" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -8190,7 +8168,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:56">
+    <row r="52" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -8225,7 +8203,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:56">
+    <row r="53" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>43</v>
       </c>
@@ -8260,7 +8238,7 @@
         <v>9.0000000000000011E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:56">
+    <row r="54" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -8295,7 +8273,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:56">
+    <row r="55" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>43</v>
       </c>
@@ -8330,7 +8308,7 @@
         <v>1.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:56">
+    <row r="56" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>43</v>
       </c>
@@ -8365,7 +8343,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:56">
+    <row r="57" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -8400,7 +8378,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:56">
+    <row r="58" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>43</v>
       </c>
@@ -8435,7 +8413,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:56">
+    <row r="59" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>43</v>
       </c>
@@ -8470,7 +8448,7 @@
         <v>9.0000000000000011E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:56">
+    <row r="60" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -8505,7 +8483,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:56">
+    <row r="61" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -8540,7 +8518,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:56">
+    <row r="62" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -8575,7 +8553,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:56">
+    <row r="63" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>43</v>
       </c>
@@ -8610,7 +8588,7 @@
         <v>1.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:56">
+    <row r="64" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>43</v>
       </c>
@@ -8645,7 +8623,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:56">
+    <row r="65" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>43</v>
       </c>
@@ -8680,7 +8658,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:56">
+    <row r="66" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -8715,7 +8693,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:56">
+    <row r="67" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -8750,7 +8728,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:56">
+    <row r="68" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>43</v>
       </c>
@@ -8785,7 +8763,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:56">
+    <row r="69" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>43</v>
       </c>
@@ -8820,7 +8798,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:56">
+    <row r="70" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>43</v>
       </c>
@@ -8855,7 +8833,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:56">
+    <row r="71" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>43</v>
       </c>
@@ -8890,7 +8868,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:56">
+    <row r="72" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>43</v>
       </c>
@@ -8925,7 +8903,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:56">
+    <row r="73" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>43</v>
       </c>
@@ -8960,7 +8938,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:56">
+    <row r="74" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>43</v>
       </c>
@@ -8995,7 +8973,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:56">
+    <row r="75" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>43</v>
       </c>
@@ -9030,7 +9008,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:56">
+    <row r="76" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>43</v>
       </c>
@@ -9065,7 +9043,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:56">
+    <row r="77" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>43</v>
       </c>
@@ -9100,7 +9078,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:56">
+    <row r="78" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>43</v>
       </c>
@@ -9135,7 +9113,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:56">
+    <row r="79" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>43</v>
       </c>
@@ -9170,7 +9148,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:56">
+    <row r="80" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>43</v>
       </c>
@@ -9205,7 +9183,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:56">
+    <row r="81" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>43</v>
       </c>
@@ -9240,7 +9218,7 @@
         <v>6.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:56">
+    <row r="82" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>43</v>
       </c>
@@ -9275,7 +9253,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:56">
+    <row r="83" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>43</v>
       </c>
@@ -9310,7 +9288,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:56">
+    <row r="84" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>43</v>
       </c>
@@ -9345,7 +9323,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:56">
+    <row r="85" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>43</v>
       </c>
@@ -9380,7 +9358,7 @@
         <v>6.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:56">
+    <row r="86" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>43</v>
       </c>
@@ -9415,7 +9393,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:56">
+    <row r="87" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>43</v>
       </c>
@@ -9450,7 +9428,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:56">
+    <row r="88" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>43</v>
       </c>
@@ -9485,7 +9463,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:56">
+    <row r="89" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>43</v>
       </c>
@@ -9520,7 +9498,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:56">
+    <row r="90" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>43</v>
       </c>
@@ -9555,7 +9533,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:56">
+    <row r="91" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>43</v>
       </c>
@@ -9590,7 +9568,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:56">
+    <row r="92" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>43</v>
       </c>
@@ -9625,7 +9603,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:56">
+    <row r="93" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>43</v>
       </c>
@@ -9660,7 +9638,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:56">
+    <row r="94" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>43</v>
       </c>
@@ -9695,7 +9673,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:56">
+    <row r="95" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>43</v>
       </c>
@@ -9730,7 +9708,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:56">
+    <row r="96" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>43</v>
       </c>
@@ -9765,7 +9743,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:56">
+    <row r="97" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>43</v>
       </c>
@@ -9800,7 +9778,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:56">
+    <row r="98" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>43</v>
       </c>
@@ -9835,7 +9813,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:56">
+    <row r="99" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>43</v>
       </c>
@@ -9870,7 +9848,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="100" spans="1:56">
+    <row r="100" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>43</v>
       </c>
@@ -9905,7 +9883,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:56">
+    <row r="101" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>43</v>
       </c>
@@ -9940,7 +9918,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:56">
+    <row r="102" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>43</v>
       </c>
@@ -9975,7 +9953,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:56">
+    <row r="103" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>43</v>
       </c>
@@ -10010,7 +9988,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:56">
+    <row r="104" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>43</v>
       </c>
@@ -10045,7 +10023,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:56">
+    <row r="105" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>43</v>
       </c>
@@ -10080,7 +10058,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:56">
+    <row r="106" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>43</v>
       </c>
@@ -10115,7 +10093,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:56">
+    <row r="107" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>43</v>
       </c>
@@ -10150,7 +10128,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:56">
+    <row r="108" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>43</v>
       </c>
@@ -10185,7 +10163,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:56">
+    <row r="109" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>43</v>
       </c>
@@ -10220,7 +10198,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:56">
+    <row r="110" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>43</v>
       </c>
@@ -10255,7 +10233,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="111" spans="1:56">
+    <row r="111" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>43</v>
       </c>
@@ -10290,7 +10268,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:56">
+    <row r="112" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>43</v>
       </c>
@@ -10331,14 +10309,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10424,7 +10402,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -10507,7 +10485,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -10566,16 +10544,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AI1" sqref="AI1:AK1"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:73" ht="52">
+    <row r="1" spans="1:73" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10679,13 +10657,13 @@
         <v>896</v>
       </c>
       <c r="AI1" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
         <v>1254</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="4" t="s">
         <v>1255</v>
-      </c>
-      <c r="AK1" s="4" t="s">
-        <v>1256</v>
       </c>
       <c r="AL1" t="s">
         <v>897</v>
@@ -10796,7 +10774,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="2" spans="1:73">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -11014,7 +10992,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="3" spans="1:73">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -11193,14 +11171,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11292,7 +11270,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -11375,7 +11353,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -11434,14 +11412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AR21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1012</v>
       </c>
@@ -11575,7 +11553,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="2" spans="1:44">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -11709,7 +11687,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="G3" t="s">
         <v>1058</v>
       </c>
@@ -11732,7 +11710,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1063</v>
       </c>
@@ -11866,7 +11844,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1096</v>
       </c>
@@ -11979,7 +11957,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1129</v>
       </c>
@@ -12080,7 +12058,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1155</v>
       </c>
@@ -12154,7 +12132,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1175</v>
       </c>
@@ -12222,7 +12200,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1192</v>
       </c>
@@ -12275,7 +12253,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1208</v>
       </c>
@@ -12307,7 +12285,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>1218</v>
       </c>
@@ -12333,7 +12311,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="H12" t="s">
         <v>1225</v>
       </c>
@@ -12350,7 +12328,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U13" t="s">
         <v>1230</v>
       </c>
@@ -12364,7 +12342,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U14" t="s">
         <v>1234</v>
       </c>
@@ -12375,7 +12353,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U15" t="s">
         <v>1237</v>
       </c>
@@ -12386,7 +12364,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U16" t="s">
         <v>1240</v>
       </c>
@@ -12397,7 +12375,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="17" spans="40:41">
+    <row r="17" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN17" t="s">
         <v>1243</v>
       </c>
@@ -12405,7 +12383,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="18" spans="40:41">
+    <row r="18" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN18" t="s">
         <v>1245</v>
       </c>
@@ -12413,7 +12391,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="19" spans="40:41">
+    <row r="19" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN19" t="s">
         <v>1247</v>
       </c>
@@ -12421,7 +12399,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="20" spans="40:41">
+    <row r="20" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN20" t="s">
         <v>1249</v>
       </c>
@@ -12429,7 +12407,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="21" spans="40:41">
+    <row r="21" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN21" t="s">
         <v>1251</v>
       </c>

</xml_diff>